<commit_message>
modified loading of sections and materials
</commit_message>
<xml_diff>
--- a/example_5_1/Example_5_1_results.xlsx
+++ b/example_5_1/Example_5_1_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Forces_D" sheetId="5" r:id="rId5"/>
     <sheet name="Member Properties" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -228,8 +228,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,11 +292,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -418,7 +413,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -453,7 +447,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -629,14 +622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -652,7 +645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -660,7 +653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -668,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -676,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -684,7 +677,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -698,12 +691,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -711,14 +704,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -726,7 +719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -734,7 +727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -742,7 +735,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -750,7 +743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -758,7 +751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -766,7 +759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -774,7 +767,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -782,7 +775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -790,7 +783,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -804,22 +797,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="8" max="8" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -857,7 +842,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -883,19 +868,19 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>9.5859406204233788E-5</v>
+        <v>9.585940620423379E-05</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>-0.18018018018018031</v>
+        <v>-0.1801801801801803</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>2</v>
       </c>
@@ -921,7 +906,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>-1.917188124084676E-4</v>
+        <v>-0.0001917188124084676</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -933,12 +918,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>359.99999999999989</v>
+        <v>359.9999999999999</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -959,24 +944,24 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>6.7101584342963642E-4</v>
+        <v>0.0006710158434296364</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>-6.9819819819819839</v>
+        <v>-6.981981981981984</v>
       </c>
       <c r="L4">
-        <v>3.2198825615804457E-14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3.219882561580446E-14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>479.99999999999989</v>
+        <v>479.9999999999999</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -997,13 +982,13 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>-2.1089069364931428E-3</v>
+        <v>-0.002108906936493143</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
       <c r="K5">
-        <v>26.081081081081091</v>
+        <v>26.08108108108109</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1015,14 +1000,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1042,7 +1027,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1053,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>-0.18018018018018031</v>
+        <v>-0.1801801801801803</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1062,7 +1047,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1073,16 +1058,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.18018018018018031</v>
+        <v>0.1801801801801803</v>
       </c>
       <c r="E3">
-        <v>-32.432432432432449</v>
+        <v>-32.43243243243245</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1093,7 +1078,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>-0.18018018018018031</v>
+        <v>-0.1801801801801803</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1102,7 +1087,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1113,16 +1098,16 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.18018018018018031</v>
+        <v>0.1801801801801803</v>
       </c>
       <c r="E5">
-        <v>-32.432432432432449</v>
+        <v>-32.43243243243245</v>
       </c>
       <c r="F5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1133,16 +1118,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.90090090090090136</v>
+        <v>0.9009009009009014</v>
       </c>
       <c r="E6">
-        <v>32.432432432432449</v>
+        <v>32.43243243243245</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1153,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-0.90090090090090136</v>
+        <v>-0.9009009009009014</v>
       </c>
       <c r="E7">
         <v>129.7297297297298</v>
@@ -1162,7 +1147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1173,16 +1158,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.90090090090090136</v>
+        <v>0.9009009009009014</v>
       </c>
       <c r="E8">
-        <v>32.432432432432449</v>
+        <v>32.43243243243245</v>
       </c>
       <c r="F8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1193,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-0.90090090090090136</v>
+        <v>-0.9009009009009014</v>
       </c>
       <c r="E9">
         <v>129.7297297297298</v>
@@ -1202,7 +1187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1213,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>-6.0810810810810816</v>
+        <v>-6.081081081081082</v>
       </c>
       <c r="E10">
         <v>-129.7297297297298</v>
@@ -1222,7 +1207,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1233,16 +1218,16 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>6.0810810810810816</v>
+        <v>6.081081081081082</v>
       </c>
       <c r="E11">
-        <v>-600.00000000000011</v>
+        <v>-600.0000000000001</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1253,7 +1238,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-6.0810810810810816</v>
+        <v>-6.081081081081082</v>
       </c>
       <c r="E12">
         <v>-129.7297297297298</v>
@@ -1262,7 +1247,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1273,10 +1258,10 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>6.0810810810810816</v>
+        <v>6.081081081081082</v>
       </c>
       <c r="E13">
-        <v>-600.00000000000011</v>
+        <v>-600.0000000000001</v>
       </c>
       <c r="F13" t="s">
         <v>55</v>
@@ -1288,14 +1273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1330,7 +1315,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1350,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>29000.000000000011</v>
+        <v>29000.00000000001</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1359,13 +1344,13 @@
         <v>10</v>
       </c>
       <c r="J2">
-        <v>350.00000000000011</v>
+        <v>350.0000000000001</v>
       </c>
       <c r="K2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1385,7 +1370,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>29000.000000000011</v>
+        <v>29000.00000000001</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1394,13 +1379,13 @@
         <v>10</v>
       </c>
       <c r="J3">
-        <v>350.00000000000011</v>
+        <v>350.0000000000001</v>
       </c>
       <c r="K3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1420,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>29000.000000000011</v>
+        <v>29000.00000000001</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1429,7 +1414,7 @@
         <v>10</v>
       </c>
       <c r="J4">
-        <v>350.00000000000011</v>
+        <v>350.0000000000001</v>
       </c>
       <c r="K4" t="s">
         <v>67</v>

</xml_diff>